<commit_message>
add a function that select the column names
</commit_message>
<xml_diff>
--- a/db_upload/info/info_table.xlsx
+++ b/db_upload/info/info_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="10580" yWindow="840" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
+    <workbookView xWindow="1460" yWindow="1020" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="133">
   <si>
     <t>db_name</t>
   </si>
@@ -416,6 +416,15 @@
   </si>
   <si>
     <t>band-width</t>
+  </si>
+  <si>
+    <t>tbl</t>
+  </si>
+  <si>
+    <t>main</t>
+  </si>
+  <si>
+    <t>param</t>
   </si>
 </sst>
 </file>
@@ -501,8 +510,56 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -549,7 +606,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="83">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -567,6 +624,30 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -584,6 +665,30 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -862,10 +967,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -873,15 +978,18 @@
     <col min="1" max="1" width="14.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>89</v>
       </c>
@@ -889,31 +997,40 @@
         <v>85</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
@@ -921,15 +1038,18 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>5</v>
       </c>
@@ -937,7 +1057,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -945,7 +1065,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -953,7 +1073,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -961,7 +1081,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>79</v>
       </c>
@@ -969,7 +1089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -977,20 +1097,26 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>84</v>
+      </c>
+      <c r="C15" t="s">
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1006,10 +1132,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B19"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C11" sqref="C11:C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1018,15 +1144,18 @@
     <col min="2" max="2" width="21.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -1034,140 +1163,191 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>18</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>63</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>20</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>21</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>23</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>24</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>67</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>68</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>25</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>27</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>28</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
       <c r="A18" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
       <c r="A19" t="s">
         <v>31</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>78</v>
+      </c>
+      <c r="C19" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1187,31 +1367,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="C6" sqref="C6:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -1219,72 +1405,97 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" t="s">
         <v>96</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>97</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>98</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>39</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1295,27 +1506,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
-    <col min="2" max="2" width="39.1640625" customWidth="1"/>
+    <col min="2" max="2" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -1323,63 +1537,84 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
         <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
         <v>50</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="8" t="s">
         <v>109</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="8" t="s">
         <v>110</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" s="7" t="s">
         <v>111</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" s="7" t="s">
         <v>48</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" s="8" t="s">
         <v>112</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" s="8" t="s">
         <v>113</v>
       </c>
@@ -1387,7 +1622,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:3">
       <c r="A11" s="8" t="s">
         <v>114</v>
       </c>
@@ -1395,7 +1630,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:3">
       <c r="A12" s="8" t="s">
         <v>54</v>
       </c>
@@ -1416,10 +1651,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1428,15 +1663,18 @@
     <col min="2" max="2" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
         <v>37</v>
       </c>
@@ -1444,7 +1682,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
         <v>47</v>
       </c>
@@ -1452,108 +1690,147 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:3">
       <c r="A4" t="s">
         <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
       <c r="A5" s="6" t="s">
         <v>125</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" s="6" t="s">
         <v>58</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>57</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
       <c r="A9" t="s">
         <v>126</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
       <c r="A10" t="s">
         <v>55</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
       <c r="A11" t="s">
         <v>127</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>119</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
       <c r="A12" t="s">
         <v>61</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
       <c r="A13" t="s">
         <v>60</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
       <c r="A14" t="s">
         <v>62</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
       <c r="A15" t="s">
         <v>128</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
       <c r="A16" t="s">
         <v>129</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>124</v>
+      </c>
+      <c r="C16" t="s">
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add upload tables person_role and publication adjusted insertion from roxas setting information "meas_date" and "calibration"
</commit_message>
<xml_diff>
--- a/db_upload/info/info_table.xlsx
+++ b/db_upload/info/info_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="160" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="2" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="year" sheetId="6" r:id="rId6"/>
     <sheet name="cell" sheetId="7" r:id="rId7"/>
     <sheet name="settings" sheetId="8" r:id="rId8"/>
+    <sheet name="publication" sheetId="9" r:id="rId9"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">cell!$A$1:$C$35</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="378" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="254">
   <si>
     <t>db_name</t>
   </si>
@@ -759,6 +760,42 @@
   </si>
   <si>
     <t>Ycal</t>
+  </si>
+  <si>
+    <t>First_author_last_name</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Journal</t>
+  </si>
+  <si>
+    <t>Doi</t>
+  </si>
+  <si>
+    <t>first_author_last_name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>journal</t>
+  </si>
+  <si>
+    <t>doi</t>
+  </si>
+  <si>
+    <t>Spatial Resolution [pixels/µm]</t>
+  </si>
+  <si>
+    <t>File created</t>
   </si>
 </sst>
 </file>
@@ -859,8 +896,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="147">
+  <cellStyleXfs count="155">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1028,7 +1073,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="147">
+  <cellStyles count="155">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1102,6 +1147,10 @@
     <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1175,6 +1224,10 @@
     <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1856,7 +1909,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection sqref="A1:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2140,7 +2193,7 @@
   <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2588,7 +2641,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
@@ -3009,10 +3062,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3039,6 +3092,22 @@
       </c>
       <c r="B3" t="s">
         <v>237</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -3049,4 +3118,88 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>248</v>
+      </c>
+      <c r="B3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>249</v>
+      </c>
+      <c r="B4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>250</v>
+      </c>
+      <c r="B5" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>251</v>
+      </c>
+      <c r="B6" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="B9" s="5"/>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="5"/>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="B11" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
correction due to error in long/lat
</commit_message>
<xml_diff>
--- a/db_upload/info/info_table.xlsx
+++ b/db_upload/info/info_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="7"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="2" r:id="rId1"/>
@@ -1498,7 +1498,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11:C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1739,8 +1739,8 @@
       <c r="A6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>32</v>
+      <c r="B6" s="1" t="s">
+        <v>33</v>
       </c>
       <c r="C6" t="s">
         <v>128</v>
@@ -1750,8 +1750,8 @@
       <c r="A7" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>33</v>
+      <c r="B7" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="C7" t="s">
         <v>128</v>
@@ -3064,7 +3064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
more little adjustments to up-load vessels
</commit_message>
<xml_diff>
--- a/db_upload/info/info_table.xlsx
+++ b/db_upload/info/info_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="257">
   <si>
     <t>db_name</t>
   </si>
@@ -796,6 +796,15 @@
   </si>
   <si>
     <t>File created</t>
+  </si>
+  <si>
+    <t>VNo</t>
+  </si>
+  <si>
+    <t>VD</t>
+  </si>
+  <si>
+    <t>vd</t>
   </si>
 </sst>
 </file>
@@ -896,8 +905,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="165">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1073,7 +1092,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="165">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1151,6 +1170,11 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1228,6 +1252,11 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1673,7 +1702,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2396,10 +2425,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2622,6 +2651,39 @@
         <v>228</v>
       </c>
       <c r="C19" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B20" t="s">
+        <v>254</v>
+      </c>
+      <c r="C20" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" t="s">
+        <v>255</v>
+      </c>
+      <c r="C21" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="8" t="s">
+        <v>148</v>
+      </c>
+      <c r="B22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C22" t="s">
         <v>194</v>
       </c>
     </row>

</xml_diff>

<commit_message>
... to up-load more sites
</commit_message>
<xml_diff>
--- a/db_upload/info/info_table.xlsx
+++ b/db_upload/info/info_table.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28125"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="2560" yWindow="0" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="person" sheetId="2" r:id="rId1"/>
@@ -905,8 +905,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="165">
+  <cellStyleXfs count="167">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1092,7 +1094,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="165">
+  <cellStyles count="167">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1175,6 +1177,7 @@
     <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1257,6 +1260,7 @@
     <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1527,7 +1531,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2221,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2427,8 +2431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2704,7 +2708,7 @@
   <dimension ref="A1:C37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A14" sqref="A14:A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>